<commit_message>
strategy and add and list
</commit_message>
<xml_diff>
--- a/public/question_sample.xlsx
+++ b/public/question_sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\React\react_tailwind_mui\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0427E036-DE62-483C-A507-A053D7F6F983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7002ABEE-F014-44E6-95E2-EDF3CD70B7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7D532751-0969-4C5D-8DB2-9408AE49EDCD}"/>
   </bookViews>
@@ -33,54 +33,146 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Candidate ID</t>
-  </si>
-  <si>
-    <t>Candidate Name</t>
-  </si>
-  <si>
-    <t>Father Name</t>
-  </si>
-  <si>
-    <t>Candidate Mobile</t>
-  </si>
-  <si>
-    <t>BFSI001</t>
-  </si>
-  <si>
-    <t>BFSI002</t>
-  </si>
-  <si>
-    <t>Candidate 1</t>
-  </si>
-  <si>
-    <t>Candidate 2</t>
-  </si>
-  <si>
-    <t>Father 1</t>
-  </si>
-  <si>
-    <t>Father 2</t>
-  </si>
-  <si>
-    <t>BFSI003</t>
-  </si>
-  <si>
-    <t>Candidate 3</t>
-  </si>
-  <si>
-    <t>Father 3</t>
-  </si>
-  <si>
-    <t>BFSI004</t>
-  </si>
-  <si>
-    <t>Candidate 4</t>
-  </si>
-  <si>
-    <t>Father 4</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+  <si>
+    <t>NOS ID</t>
+  </si>
+  <si>
+    <t>PC Number</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Correct Option
+Ex: 1,2,3,4</t>
+  </si>
+  <si>
+    <t>Option 1</t>
+  </si>
+  <si>
+    <t>Option 2</t>
+  </si>
+  <si>
+    <t>Option 3</t>
+  </si>
+  <si>
+    <t>Option 4</t>
+  </si>
+  <si>
+    <t>Language Question</t>
+  </si>
+  <si>
+    <t>Language Description</t>
+  </si>
+  <si>
+    <t>Language Option 1</t>
+  </si>
+  <si>
+    <t>Language Option 2</t>
+  </si>
+  <si>
+    <t>Language Option 3</t>
+  </si>
+  <si>
+    <t>Language Option 4</t>
+  </si>
+  <si>
+    <t>eng=English
+hin=Hindi
+mar=Marathi
+guj=Gujrati
+mal=Malayalam
+pan=Punjabi
+asm=Assamese
+ori=Odia
+ben=Bengali
+tel=Telugu</t>
+  </si>
+  <si>
+    <t>Question type
+1=Multiple Choice
+2=VIVA
+3=DEMO</t>
+  </si>
+  <si>
+    <t>What is the function of a balance wheel in a sewing machine?</t>
+  </si>
+  <si>
+    <t>To run or stop the machine</t>
+  </si>
+  <si>
+    <t>To control the movement of the needle</t>
+  </si>
+  <si>
+    <t>To guide the thread from the spool to the needle</t>
+  </si>
+  <si>
+    <t>To hold the presser foot</t>
+  </si>
+  <si>
+    <t>hin</t>
+  </si>
+  <si>
+    <t>सिलाई मशीन में बैलेंस व्हील का क्या कार्य है?</t>
+  </si>
+  <si>
+    <t>मशीन को चलाने या रोकने के लिए</t>
+  </si>
+  <si>
+    <t>रील से सुई तक धागे का मार्गदर्शन करने के लिए</t>
+  </si>
+  <si>
+    <t>प्रेसर फुट को पकड़ने क लिए</t>
+  </si>
+  <si>
+    <t>What is the function of a thread stand in a sewing machine?</t>
+  </si>
+  <si>
+    <t>To wind the bottom thread</t>
+  </si>
+  <si>
+    <t>To catch the top thread for stitching</t>
+  </si>
+  <si>
+    <t>To hold the thread pool for stitching</t>
+  </si>
+  <si>
+    <t>To hold the material for stitching</t>
+  </si>
+  <si>
+    <t>सिलाई के लिए ऊपरी धागे को पकड़ने के लिए</t>
+  </si>
+  <si>
+    <t>सिलाई मशीन में थ्रेड स्टैंड का क्या कार्य है?</t>
+  </si>
+  <si>
+    <t>MEP/N7101</t>
+  </si>
+  <si>
+    <t>MEP/N7102</t>
+  </si>
+  <si>
+    <t>नीचे के धागे को लपेटने के लिए</t>
+  </si>
+  <si>
+    <t>सिलाई के लिए धागा पूल पकड़ने के लिए</t>
+  </si>
+  <si>
+    <t>सिलाई के लिए मैटेरियल पकड़ने के लिए</t>
+  </si>
+  <si>
+    <t>Difficulty Level
+level 1
+level 2
+level 3
+level 4</t>
+  </si>
+  <si>
+    <t>level 4</t>
   </si>
 </sst>
 </file>
@@ -135,9 +227,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -153,6 +248,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1572904</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1243692</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDE4B734-6767-49CA-9A85-9A509629EF14}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2181225" y="1905000"/>
+          <a:ext cx="1572904" cy="1243692"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -452,93 +596,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445D52A1-996F-4CDA-A157-41471B47C950}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="150" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>8936475836</v>
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>8936475837</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>8936475838</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5">
-        <v>8936475839</v>
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
strategy add, edit and details with element in jobroles and questions
</commit_message>
<xml_diff>
--- a/public/question_sample.xlsx
+++ b/public/question_sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\React\react_tailwind_mui\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7002ABEE-F014-44E6-95E2-EDF3CD70B7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649EF8B4-7517-41D1-9618-99DCB81B2C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7D532751-0969-4C5D-8DB2-9408AE49EDCD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>NOS ID</t>
   </si>
@@ -173,6 +173,15 @@
   </si>
   <si>
     <t>level 4</t>
+  </si>
+  <si>
+    <t>Element</t>
+  </si>
+  <si>
+    <t>MEP/N7101-1</t>
+  </si>
+  <si>
+    <t>MEP/N7102-1</t>
   </si>
 </sst>
 </file>
@@ -254,13 +263,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>1572904</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>1243692</xdr:rowOff>
@@ -596,186 +605,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445D52A1-996F-4CDA-A157-41471B47C950}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="39" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>42</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>40</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>23</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>24</v>
-      </c>
-      <c r="P2" t="s">
-        <v>25</v>
       </c>
       <c r="Q2" t="s">
         <v>25</v>
       </c>
       <c r="R2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>43</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>27</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>28</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>29</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>30</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>31</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>40</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>22</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>33</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>36</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>37</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>